<commit_message>
rp serialization still needs unserialization
</commit_message>
<xml_diff>
--- a/Fall_Quarter_Gantt_2016.xlsx
+++ b/Fall_Quarter_Gantt_2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Start Date</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Tasks</t>
+  </si>
+  <si>
+    <t>Route Prediction Data Serialization</t>
   </si>
 </sst>
 </file>
@@ -262,18 +265,6 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
             <c:idx val="10"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -309,11 +300,23 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Route Prediction Working</c:v>
                 </c:pt>
@@ -339,18 +342,21 @@
                   <c:v>main.cpp</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Route Prediction Data Serialization</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Gather Road Data / Validate</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Make Presentation</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Write Thesis</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Code Clean-up</c:v>
                 </c:pt>
               </c:strCache>
@@ -358,10 +364,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0" formatCode="m/d/yy">
                   <c:v>42619.0</c:v>
                 </c:pt>
@@ -383,16 +389,19 @@
                 <c:pt idx="7" formatCode="m/d/yy">
                   <c:v>42659.0</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="m/d/yy">
+                <c:pt idx="8" formatCode="m/d/yy">
+                  <c:v>42658.0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="m/d/yy">
                   <c:v>42668.0</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="m/d/yy">
+                <c:pt idx="11" formatCode="m/d/yy">
                   <c:v>42689.0</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="m/d/yy">
+                <c:pt idx="12" formatCode="m/d/yy">
                   <c:v>42675.0</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="m/d/yy">
+                <c:pt idx="13" formatCode="m/d/yy">
                   <c:v>42675.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -417,9 +426,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Route Prediction Working</c:v>
                 </c:pt>
@@ -445,18 +454,21 @@
                   <c:v>main.cpp</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Route Prediction Data Serialization</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Gather Road Data / Validate</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Make Presentation</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Write Thesis</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Code Clean-up</c:v>
                 </c:pt>
               </c:strCache>
@@ -464,10 +476,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>10.0</c:v>
                 </c:pt>
@@ -493,18 +505,21 @@
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>14.0</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>24.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -521,11 +536,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2119389728"/>
-        <c:axId val="-2095712576"/>
+        <c:axId val="-2104627664"/>
+        <c:axId val="-2104624304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119389728"/>
+        <c:axId val="-2104627664"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -568,7 +583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095712576"/>
+        <c:crossAx val="-2104624304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095712576"/>
+        <c:axId val="-2104624304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42705.0"/>
@@ -629,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119389728"/>
+        <c:crossAx val="-2104627664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1261,13 +1276,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1435100</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1553,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1597,7 +1612,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1605,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D15" si="0">C3-B3</f>
         <v>0</v>
       </c>
       <c r="E3" s="1">
@@ -1645,7 +1660,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1722,29 +1737,29 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42658</v>
+      </c>
+      <c r="C10" s="2">
+        <v>42668</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
-        <v>42668</v>
-      </c>
-      <c r="C11" s="2">
-        <v>42675</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -1752,35 +1767,35 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>42689</v>
+        <v>42668</v>
       </c>
       <c r="C12" s="2">
-        <v>42699</v>
+        <v>42675</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
-        <v>42675</v>
+        <v>42689</v>
       </c>
       <c r="C13" s="2">
-        <v>42689</v>
+        <v>42699</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1">
         <v>0.15</v>
@@ -1788,19 +1803,37 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2">
         <v>42675</v>
       </c>
       <c r="C14" s="2">
-        <v>42699</v>
+        <v>42689</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>42675</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42699</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working vehicle modeling kinematics
</commit_message>
<xml_diff>
--- a/Fall_Quarter_Gantt_2016.xlsx
+++ b/Fall_Quarter_Gantt_2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12480" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="15420" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>Route Prediction Data Serialization</t>
+    <t>Driver Prediction Data Serialization</t>
   </si>
 </sst>
 </file>
@@ -193,6 +193,18 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -265,6 +277,18 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="10"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -342,7 +366,7 @@
                   <c:v>main.cpp</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Route Prediction Data Serialization</c:v>
+                  <c:v>Driver Prediction Data Serialization</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
@@ -366,42 +390,45 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="m/d/yy">
+                <c:pt idx="0">
                   <c:v>42619.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="m/d/yy">
+                <c:pt idx="1">
+                  <c:v>42661.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>42653.0</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="m/d/yy">
+                <c:pt idx="3">
                   <c:v>42633.0</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="m/d/yy">
+                <c:pt idx="4">
                   <c:v>42639.0</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="m/d/yy">
+                <c:pt idx="5">
                   <c:v>42644.0</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="m/d/yy">
+                <c:pt idx="6">
                   <c:v>42650.0</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="m/d/yy">
+                <c:pt idx="7">
                   <c:v>42659.0</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="m/d/yy">
+                <c:pt idx="8">
                   <c:v>42658.0</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="m/d/yy">
+                <c:pt idx="10">
                   <c:v>42668.0</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="m/d/yy">
+                <c:pt idx="11">
                   <c:v>42689.0</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="m/d/yy">
+                <c:pt idx="12">
                   <c:v>42675.0</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="m/d/yy">
+                <c:pt idx="13">
                   <c:v>42675.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -454,7 +481,7 @@
                   <c:v>main.cpp</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Route Prediction Data Serialization</c:v>
+                  <c:v>Driver Prediction Data Serialization</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
@@ -484,7 +511,7 @@
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
@@ -505,7 +532,7 @@
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
@@ -536,11 +563,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2104627664"/>
-        <c:axId val="-2104624304"/>
+        <c:axId val="-2078545280"/>
+        <c:axId val="-2078541936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2104627664"/>
+        <c:axId val="-2078545280"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -583,7 +610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104624304"/>
+        <c:crossAx val="-2078541936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -591,7 +618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104624304"/>
+        <c:axId val="-2078541936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42705.0"/>
@@ -644,7 +671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104627664"/>
+        <c:crossAx val="-2078545280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1571,7 +1598,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1619,9 +1646,15 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="2">
+        <v>42661</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42662</v>
+      </c>
       <c r="D3">
         <f t="shared" ref="D3:D15" si="0">C3-B3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1696,7 +1729,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1714,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1743,14 +1776,14 @@
         <v>42658</v>
       </c>
       <c r="C10" s="2">
-        <v>42668</v>
+        <v>42663</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>C10-B10</f>
+        <v>5</v>
       </c>
       <c r="E10" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
GPS input parser complete
</commit_message>
<xml_diff>
--- a/Fall_Quarter_Gantt_2016.xlsx
+++ b/Fall_Quarter_Gantt_2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="15420" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="15420" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1598,7 +1598,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
road / intersection deviation complete
</commit_message>
<xml_diff>
--- a/Fall_Quarter_Gantt_2016.xlsx
+++ b/Fall_Quarter_Gantt_2016.xlsx
@@ -41,9 +41,6 @@
     <t>GPS Input Parser</t>
   </si>
   <si>
-    <t>GPS Road Deviation</t>
-  </si>
-  <si>
     <t>Road-Load Kinematics Model</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Driver Prediction Data Serialization</t>
+  </si>
+  <si>
+    <t>GPS Road / Intersection Deviation</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
                   <c:v>GPS Input Parser</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>GPS Road Deviation</c:v>
+                  <c:v>GPS Road / Intersection Deviation</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Map Spline Intersection Working</c:v>
@@ -463,7 +463,7 @@
                   <c:v>GPS Input Parser</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>GPS Road Deviation</c:v>
+                  <c:v>GPS Road / Intersection Deviation</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Map Spline Intersection Working</c:v>
@@ -1598,7 +1598,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1609,7 +1609,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1618,15 +1618,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2">
         <v>42619</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
         <v>42653</v>
@@ -1675,12 +1675,12 @@
         <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>42633</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>42650</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>42659</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <v>42658</v>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <v>42668</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>42689</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>42675</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2">
         <v>42675</v>

</xml_diff>

<commit_message>
driver prediction mostly done
</commit_message>
<xml_diff>
--- a/Fall_Quarter_Gantt_2016.xlsx
+++ b/Fall_Quarter_Gantt_2016.xlsx
@@ -44,9 +44,6 @@
     <t>Road-Load Kinematics Model</t>
   </si>
   <si>
-    <t>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</t>
-  </si>
-  <si>
     <t>Make Presentation</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>GPS Road / Intersection Deviation</t>
+  </si>
+  <si>
+    <t>OBD2 Parser Speed-&gt;NN / Fuel-Flow-&gt;Log</t>
   </si>
 </sst>
 </file>
@@ -345,40 +345,40 @@
                   <c:v>Route Prediction Working</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Map Spline Intersection Working</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Improved Elevation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Road-Load Kinematics Model</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>GPS Input Parser</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>Driver Prediction Data Serialization</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>GPS Road / Intersection Deviation</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Map Spline Intersection Working</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Driver Prediction ML Wrapper</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Improved Elevation</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Road-Load Kinematics Model</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>main.cpp</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Driver Prediction Data Serialization</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
+                  <c:v>OBD2 Parser Speed-&gt;NN / Fuel-Flow-&gt;Log</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Gather Road Data / Validate</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Write Thesis</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Make Presentation</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Write Thesis</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Code Clean-up</c:v>
@@ -396,37 +396,37 @@
                   <c:v>42619.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>42629.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42644.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42650.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42658.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42658.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>42661.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>42653.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42633.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42639.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42644.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42650.0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>42659.0</c:v>
+                  <c:v>42663.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42658.0</c:v>
+                  <c:v>42663.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42668.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>42675.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>42689.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42675.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>42675.0</c:v>
@@ -460,40 +460,40 @@
                   <c:v>Route Prediction Working</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Map Spline Intersection Working</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Improved Elevation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Road-Load Kinematics Model</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>GPS Input Parser</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>Driver Prediction Data Serialization</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>GPS Road / Intersection Deviation</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Map Spline Intersection Working</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Driver Prediction ML Wrapper</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Improved Elevation</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Road-Load Kinematics Model</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>main.cpp</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Driver Prediction Data Serialization</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>OBD2 Parser Speed-&gt;NN / FF-&gt;Log</c:v>
+                  <c:v>OBD2 Parser Speed-&gt;NN / Fuel-Flow-&gt;Log</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Gather Road Data / Validate</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Write Thesis</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Make Presentation</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Write Thesis</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Code Clean-up</c:v>
@@ -511,16 +511,16 @@
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.0</c:v>
@@ -529,7 +529,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.0</c:v>
@@ -541,10 +541,10 @@
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>24.0</c:v>
@@ -1598,18 +1598,18 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1618,15 +1618,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>42619</v>
@@ -1644,17 +1644,17 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>42661</v>
+        <v>42629</v>
       </c>
       <c r="C3" s="2">
-        <v>42662</v>
+        <v>42638</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D15" si="0">C3-B3</f>
-        <v>1</v>
+        <f>C3-B3</f>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1662,16 +1662,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>42653</v>
+        <v>42644</v>
       </c>
       <c r="C4" s="2">
-        <v>42658</v>
+        <v>42649</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>C4-B4</f>
         <v>5</v>
       </c>
       <c r="E4" s="1">
@@ -1680,17 +1680,17 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>42633</v>
+        <v>42650</v>
       </c>
       <c r="C5" s="2">
-        <v>42638</v>
+        <v>42652</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C5-B5</f>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1698,34 +1698,34 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>42639</v>
+        <v>42658</v>
       </c>
       <c r="C6" s="2">
-        <v>42643</v>
+        <v>42659</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="D6:D15" si="0">C6-B6</f>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>42644</v>
+        <v>42658</v>
       </c>
       <c r="C7" s="2">
-        <v>42649</v>
+        <v>42663</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>C7-B7</f>
         <v>5</v>
       </c>
       <c r="E7" s="1">
@@ -1734,13 +1734,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
-        <v>42650</v>
+        <v>42661</v>
       </c>
       <c r="C8" s="2">
-        <v>42652</v>
+        <v>42663</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -1752,17 +1752,17 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
-        <v>42659</v>
+        <v>42663</v>
       </c>
       <c r="C9" s="2">
         <v>42668</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1770,25 +1770,25 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
-        <v>42658</v>
+        <v>42663</v>
       </c>
       <c r="C10" s="2">
-        <v>42663</v>
+        <v>42668</v>
       </c>
       <c r="D10">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>42668</v>
@@ -1821,14 +1821,14 @@
         <v>7</v>
       </c>
       <c r="B13" s="2">
+        <v>42675</v>
+      </c>
+      <c r="C13" s="2">
         <v>42689</v>
       </c>
-      <c r="C13" s="2">
-        <v>42699</v>
-      </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>C13-B13</f>
+        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>0.15</v>
@@ -1836,17 +1836,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>42675</v>
+        <v>42689</v>
       </c>
       <c r="C14" s="2">
-        <v>42689</v>
+        <v>42699</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1">
         <v>0.15</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>42675</v>

</xml_diff>